<commit_message>
Prepare for MT, but slower than slow
</commit_message>
<xml_diff>
--- a/BenchProfRunnSum.xlsx
+++ b/BenchProfRunnSum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="20730" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t xml:space="preserve"> Init     </t>
   </si>
@@ -136,6 +137,27 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>A200</t>
+  </si>
+  <si>
+    <t>Multithread, but not thread safe…</t>
+  </si>
+  <si>
+    <t>The out is wrong</t>
+  </si>
+  <si>
+    <t>A201</t>
+  </si>
+  <si>
+    <t>Single TH, but safe. GPU style</t>
+  </si>
+  <si>
+    <t>A203</t>
+  </si>
+  <si>
+    <t>Out ok</t>
   </si>
 </sst>
 </file>
@@ -143,7 +165,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -535,85 +557,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,34 +940,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -957,19 +983,34 @@
       <c r="D2">
         <v>40000</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2">
+        <v>40000</v>
+      </c>
+      <c r="F2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="29" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="29" t="s">
         <v>12</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -985,24 +1026,33 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1016,6 +1066,15 @@
       </c>
       <c r="D6">
         <v>1</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1031,6 +1090,15 @@
       <c r="D7">
         <v>349</v>
       </c>
+      <c r="E7">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>3426</v>
+      </c>
+      <c r="G7">
+        <v>8810</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1045,6 +1113,15 @@
       <c r="D8">
         <v>1566</v>
       </c>
+      <c r="E8">
+        <v>183</v>
+      </c>
+      <c r="F8">
+        <v>1556</v>
+      </c>
+      <c r="G8">
+        <v>6944</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1064,15 +1141,15 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>216</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4984</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15756</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
@@ -1093,6 +1170,17 @@
       <c r="L9">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1108,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,372 +1206,372 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>182</v>
       </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
         <v>100</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>179</v>
       </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
         <v>98.35</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>179</v>
       </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
         <v>98.35</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>96</v>
       </c>
-      <c r="C5" s="10">
-        <v>0</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
         <v>52.75</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>82</v>
       </c>
-      <c r="C6" s="15">
-        <v>0</v>
-      </c>
-      <c r="D6" s="15">
+      <c r="C6" s="14">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14">
         <v>45.05</v>
       </c>
-      <c r="E6" s="16">
-        <v>0</v>
-      </c>
-      <c r="F6" s="26">
+      <c r="E6" s="15">
+        <v>0</v>
+      </c>
+      <c r="F6" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>82</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>4</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>45.05</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="15">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="26">
         <f>E7/D6*100</f>
         <v>4.8834628190899014</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="17">
         <v>24</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <v>8</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>13.19</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="18">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="27">
         <f>D8/$D$6*100</f>
         <v>29.278579356270811</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="20">
         <v>14</v>
       </c>
-      <c r="C9" s="21">
-        <v>0</v>
-      </c>
-      <c r="D9" s="21">
+      <c r="C9" s="20">
+        <v>0</v>
+      </c>
+      <c r="D9" s="20">
         <v>7.69</v>
       </c>
-      <c r="E9" s="22">
-        <v>0</v>
-      </c>
-      <c r="F9" s="28">
+      <c r="E9" s="21">
+        <v>0</v>
+      </c>
+      <c r="F9" s="27">
         <f t="shared" ref="F9:F16" si="0">D9/$D$6*100</f>
         <v>17.069922308546062</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <v>13</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="20">
         <v>1</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>7.14</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="21">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="27">
         <f t="shared" si="0"/>
         <v>15.849056603773585</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="20">
         <v>11</v>
       </c>
-      <c r="C11" s="21">
-        <v>0</v>
-      </c>
-      <c r="D11" s="21">
+      <c r="C11" s="20">
+        <v>0</v>
+      </c>
+      <c r="D11" s="20">
         <v>6.04</v>
       </c>
-      <c r="E11" s="22">
-        <v>0</v>
-      </c>
-      <c r="F11" s="28">
+      <c r="E11" s="21">
+        <v>0</v>
+      </c>
+      <c r="F11" s="27">
         <f t="shared" si="0"/>
         <v>13.407325194228637</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>7</v>
       </c>
-      <c r="C12" s="21">
-        <v>0</v>
-      </c>
-      <c r="D12" s="21">
+      <c r="C12" s="20">
+        <v>0</v>
+      </c>
+      <c r="D12" s="20">
         <v>3.85</v>
       </c>
-      <c r="E12" s="22">
-        <v>0</v>
-      </c>
-      <c r="F12" s="28">
+      <c r="E12" s="21">
+        <v>0</v>
+      </c>
+      <c r="F12" s="27">
         <f t="shared" si="0"/>
         <v>8.5460599334073262</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="20">
         <v>4</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="20">
         <v>1</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="21">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="27">
         <f t="shared" si="0"/>
         <v>4.8834628190899014</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="20">
         <v>2</v>
       </c>
-      <c r="C14" s="21">
-        <v>0</v>
-      </c>
-      <c r="D14" s="21">
+      <c r="C14" s="20">
+        <v>0</v>
+      </c>
+      <c r="D14" s="20">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E14" s="22">
-        <v>0</v>
-      </c>
-      <c r="F14" s="28">
+      <c r="E14" s="21">
+        <v>0</v>
+      </c>
+      <c r="F14" s="27">
         <f t="shared" si="0"/>
         <v>2.4417314095449507</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="20">
         <v>2</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="20">
         <v>2</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="20">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="26">
         <f t="shared" si="0"/>
         <v>2.4417314095449507</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>1</v>
       </c>
-      <c r="C16" s="24">
-        <v>0</v>
-      </c>
-      <c r="D16" s="24">
+      <c r="C16" s="23">
+        <v>0</v>
+      </c>
+      <c r="D16" s="23">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E16" s="25">
-        <v>0</v>
-      </c>
-      <c r="F16" s="28">
+      <c r="E16" s="24">
+        <v>0</v>
+      </c>
+      <c r="F16" s="27">
         <f t="shared" si="0"/>
         <v>1.2208657047724754</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="28">
         <f>SUM(F8:F14)+F16</f>
         <v>92.697003329633745</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="74.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <v>1</v>
       </c>
-      <c r="C17" s="12">
-        <v>0</v>
-      </c>
-      <c r="D17" s="12">
+      <c r="C17" s="11">
+        <v>0</v>
+      </c>
+      <c r="D17" s="11">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>3</v>
       </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
         <v>1.65</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>3</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>3</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>1.65</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>1.65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RFR: step_time() output has some bug...
</commit_message>
<xml_diff>
--- a/BenchProfRunnSum.xlsx
+++ b/BenchProfRunnSum.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="20730" windowHeight="11700"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="20730" windowHeight="11640" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="A102" sheetId="2" r:id="rId2"/>
     <sheet name="A203" sheetId="3" r:id="rId3"/>
     <sheet name="A204" sheetId="4" r:id="rId4"/>
+    <sheet name="A302" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="91">
   <si>
     <t xml:space="preserve"> Init     </t>
   </si>
@@ -237,6 +237,60 @@
   </si>
   <si>
     <t xml:space="preserve">  NetFlow::__find_nearest_earlier_index__</t>
+  </si>
+  <si>
+    <t>First version of refactored step_time()</t>
+  </si>
+  <si>
+    <t>Single thread</t>
+  </si>
+  <si>
+    <t>4 threds</t>
+  </si>
+  <si>
+    <t>A301</t>
+  </si>
+  <si>
+    <t>A302</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  SimRunnerThread::step_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    SimRunnerThread::need_to_rerun_ts_ansi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Barrier::synch_threads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Barrier::synch_threads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CPrimitives::X_CARRY4::calculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CPrimitives::X_SFF::calculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    NetFlow::set_at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    calculate_BUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    NetFlow::step_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CPrimitives::X_LUT6::calculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CPrimitives::X_LUT5::calculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Barrier::synch_threads</t>
   </si>
 </sst>
 </file>
@@ -314,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -632,11 +686,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -715,23 +812,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1036,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,24 +1154,25 @@
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1109,6 +1219,12 @@
       <c r="H3" s="29" t="s">
         <v>67</v>
       </c>
+      <c r="I3" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="29" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1134,6 +1250,12 @@
       </c>
       <c r="H4" t="s">
         <v>66</v>
+      </c>
+      <c r="I4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1179,6 +1301,12 @@
       <c r="H6">
         <v>1</v>
       </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1204,6 +1332,12 @@
       </c>
       <c r="H7">
         <v>660</v>
+      </c>
+      <c r="I7">
+        <v>192</v>
+      </c>
+      <c r="J7">
+        <v>909</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1231,6 +1365,12 @@
       <c r="H8">
         <v>1914</v>
       </c>
+      <c r="I8">
+        <v>1021</v>
+      </c>
+      <c r="J8">
+        <v>1039</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1266,11 +1406,11 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1214</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1949</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
@@ -1293,6 +1433,12 @@
       </c>
       <c r="H10" t="s">
         <v>67</v>
+      </c>
+      <c r="I10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1732,7 +1878,7 @@
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="30">
         <v>2269</v>
       </c>
       <c r="D2" s="2">
@@ -1752,7 +1898,7 @@
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="30">
         <v>2263</v>
       </c>
       <c r="D3" s="2">
@@ -1772,7 +1918,7 @@
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="30">
         <v>1459</v>
       </c>
       <c r="D4" s="2">
@@ -2025,7 +2171,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>55</v>
       </c>
@@ -2045,7 +2191,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>56</v>
       </c>
@@ -2065,7 +2211,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2085,7 +2231,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>58</v>
       </c>
@@ -2125,7 +2271,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>60</v>
       </c>
@@ -2145,7 +2291,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>61</v>
       </c>
@@ -2165,7 +2311,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -2185,7 +2331,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -2205,7 +2351,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>64</v>
       </c>
@@ -2225,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>65</v>
       </c>
@@ -2245,7 +2391,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>64</v>
       </c>
@@ -2265,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>65</v>
       </c>
@@ -2296,7 +2442,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,87 +2485,87 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="31">
         <v>132</v>
       </c>
-      <c r="C3" s="32">
-        <v>1</v>
-      </c>
-      <c r="D3" s="32">
+      <c r="C3" s="31">
+        <v>1</v>
+      </c>
+      <c r="D3" s="31">
         <v>52.17</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="32">
         <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="31">
         <v>34</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="31">
         <v>3</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <v>13.44</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="32">
         <v>1.19</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="31">
         <v>23</v>
       </c>
-      <c r="C5" s="32">
-        <v>0</v>
-      </c>
-      <c r="D5" s="32">
+      <c r="C5" s="31">
+        <v>0</v>
+      </c>
+      <c r="D5" s="31">
         <v>9.09</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="31">
         <v>18</v>
       </c>
-      <c r="C6" s="32">
-        <v>0</v>
-      </c>
-      <c r="D6" s="32">
+      <c r="C6" s="31">
+        <v>0</v>
+      </c>
+      <c r="D6" s="31">
         <v>7.11</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <v>18</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <v>5</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <v>7.11</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="32">
         <v>1.98</v>
       </c>
     </row>
@@ -2458,125 +2604,424 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="31">
         <v>16</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>2</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <v>6.32</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="32">
         <v>0.79</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="31">
         <v>13</v>
       </c>
-      <c r="C11" s="32">
-        <v>1</v>
-      </c>
-      <c r="D11" s="32">
+      <c r="C11" s="31">
+        <v>1</v>
+      </c>
+      <c r="D11" s="31">
         <v>5.14</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="32">
         <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="31">
         <v>12</v>
       </c>
-      <c r="C12" s="32">
-        <v>1</v>
-      </c>
-      <c r="D12" s="32">
+      <c r="C12" s="31">
+        <v>1</v>
+      </c>
+      <c r="D12" s="31">
         <v>4.74</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="32">
         <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="31">
         <v>7</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="31">
         <v>2</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="31">
         <v>2.77</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="32">
         <v>0.79</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="31">
         <v>5</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="31">
         <v>5</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="31">
         <v>1.98</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="32">
         <v>1.98</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="31">
         <v>2</v>
       </c>
-      <c r="C15" s="32">
-        <v>0</v>
-      </c>
-      <c r="D15" s="32">
+      <c r="C15" s="31">
+        <v>0</v>
+      </c>
+      <c r="D15" s="31">
         <v>0.79</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="34">
-        <v>1</v>
-      </c>
-      <c r="C16" s="34">
-        <v>0</v>
-      </c>
-      <c r="D16" s="34">
+      <c r="B16" s="33">
+        <v>1</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0</v>
+      </c>
+      <c r="D16" s="33">
         <v>0.4</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16" s="34">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="2">
+        <v>554</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>88.92</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="2">
+        <v>346</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>55.54</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="2">
+        <v>217</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>34.83</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="2">
+        <v>216</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>34.67</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="2">
+        <v>90</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>14.45</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="36"/>
+      <c r="B11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="6">
+        <v>208</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>33.39</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FIX: RERUN when it should. OUT is OK
</commit_message>
<xml_diff>
--- a/BenchProfRunnSum.xlsx
+++ b/BenchProfRunnSum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="20730" windowHeight="11640" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="20730" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
   <si>
     <t xml:space="preserve"> Init     </t>
   </si>
@@ -146,9 +146,6 @@
     <t>Multithread, but not thread safe…</t>
   </si>
   <si>
-    <t>The out is wrong</t>
-  </si>
-  <si>
     <t>A201</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>A203</t>
   </si>
   <si>
-    <t>Out ok</t>
-  </si>
-  <si>
     <t>Module Name</t>
   </si>
   <si>
@@ -291,6 +285,36 @@
   </si>
   <si>
     <t xml:space="preserve">  Barrier::synch_threads</t>
+  </si>
+  <si>
+    <t>Barriers</t>
+  </si>
+  <si>
+    <t>The out is totally wrong</t>
+  </si>
+  <si>
+    <t>Out is better</t>
+  </si>
+  <si>
+    <t>OUT is wrong</t>
+  </si>
+  <si>
+    <t>Fixed out</t>
+  </si>
+  <si>
+    <t>A401</t>
+  </si>
+  <si>
+    <t>1TH</t>
+  </si>
+  <si>
+    <t>A402</t>
+  </si>
+  <si>
+    <t>4Th</t>
+  </si>
+  <si>
+    <t>OUT is OK</t>
   </si>
 </sst>
 </file>
@@ -330,7 +354,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,8 +391,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -729,11 +759,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -842,11 +881,49 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1143,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,10 +1258,10 @@
       <c r="B2">
         <v>4000</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="42">
         <v>4000</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="42">
         <v>40000</v>
       </c>
       <c r="E2">
@@ -1198,32 +1275,35 @@
       <c r="A3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="29" t="s">
-        <v>67</v>
+      <c r="F3" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>65</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="J3" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="41" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1243,19 +1323,25 @@
         <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="K4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1307,6 +1393,12 @@
       <c r="J6">
         <v>1</v>
       </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1338,6 +1430,12 @@
       </c>
       <c r="J7">
         <v>909</v>
+      </c>
+      <c r="K7">
+        <v>203</v>
+      </c>
+      <c r="L7">
+        <v>807</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1371,6 +1469,12 @@
       <c r="J8">
         <v>1039</v>
       </c>
+      <c r="K8">
+        <v>1514</v>
+      </c>
+      <c r="L8">
+        <v>1485</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1414,36 +1518,58 @@
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1718</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" t="s">
-        <v>75</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="L10" s="42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E11" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B1:K1"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="K11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1856,7 +1982,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>18</v>
@@ -1873,7 +1999,7 @@
     </row>
     <row r="2" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
@@ -1893,7 +2019,7 @@
     </row>
     <row r="3" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
@@ -1913,7 +2039,7 @@
     </row>
     <row r="4" spans="1:6" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>22</v>
@@ -2053,7 +2179,7 @@
     </row>
     <row r="11" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>22</v>
@@ -2093,7 +2219,7 @@
     </row>
     <row r="13" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>22</v>
@@ -2133,7 +2259,7 @@
     </row>
     <row r="15" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>22</v>
@@ -2153,7 +2279,7 @@
     </row>
     <row r="16" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>22</v>
@@ -2173,7 +2299,7 @@
     </row>
     <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>22</v>
@@ -2193,7 +2319,7 @@
     </row>
     <row r="18" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>22</v>
@@ -2213,7 +2339,7 @@
     </row>
     <row r="19" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>22</v>
@@ -2233,7 +2359,7 @@
     </row>
     <row r="20" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>22</v>
@@ -2253,7 +2379,7 @@
     </row>
     <row r="21" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
@@ -2273,7 +2399,7 @@
     </row>
     <row r="22" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>22</v>
@@ -2293,7 +2419,7 @@
     </row>
     <row r="23" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>22</v>
@@ -2313,7 +2439,7 @@
     </row>
     <row r="24" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>22</v>
@@ -2333,7 +2459,7 @@
     </row>
     <row r="25" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>22</v>
@@ -2353,7 +2479,7 @@
     </row>
     <row r="26" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>22</v>
@@ -2373,7 +2499,7 @@
     </row>
     <row r="27" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>22</v>
@@ -2393,7 +2519,7 @@
     </row>
     <row r="28" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>22</v>
@@ -2413,7 +2539,7 @@
     </row>
     <row r="29" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>22</v>
@@ -2469,7 +2595,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2">
         <v>132</v>
@@ -2486,7 +2612,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="31">
         <v>132</v>
@@ -2554,7 +2680,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B7" s="31">
         <v>18</v>
@@ -2571,7 +2697,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" s="2">
         <v>11</v>
@@ -2588,7 +2714,7 @@
     </row>
     <row r="9" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
@@ -2656,7 +2782,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" s="31">
         <v>7</v>
@@ -2673,7 +2799,7 @@
     </row>
     <row r="14" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" s="31">
         <v>5</v>
@@ -2690,7 +2816,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B15" s="31">
         <v>2</v>
@@ -2729,19 +2855,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
         <v>17</v>
       </c>
@@ -2759,12 +2886,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2">
         <v>554</v>
@@ -2778,13 +2905,21 @@
       <c r="F2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" t="b">
+        <f>ISNUMBER(FIND("Barrier", B2))</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>IF(G2, E2, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2">
         <v>346</v>
@@ -2798,13 +2933,21 @@
       <c r="F3" s="5">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" t="b">
+        <f t="shared" ref="G3:G14" si="0">ISNUMBER(FIND("Barrier", B3))</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H14" si="1">IF(G3, E3, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" s="2">
         <v>217</v>
@@ -2818,13 +2961,21 @@
       <c r="F4" s="5">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2">
         <v>216</v>
@@ -2838,13 +2989,21 @@
       <c r="F5" s="5">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>34.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" s="2">
         <v>90</v>
@@ -2858,13 +3017,21 @@
       <c r="F6" s="5">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>14.45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" s="2">
         <v>7</v>
@@ -2878,13 +3045,21 @@
       <c r="F7" s="5">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G7" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2">
         <v>7</v>
@@ -2898,13 +3073,21 @@
       <c r="F8" s="5">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" s="2">
         <v>6</v>
@@ -2918,13 +3101,21 @@
       <c r="F9" s="5">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C10" s="2">
         <v>5</v>
@@ -2938,11 +3129,19 @@
       <c r="F10" s="5">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36"/>
       <c r="B11" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="2">
         <v>5</v>
@@ -2956,13 +3155,21 @@
       <c r="F11" s="5">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C12" s="2">
         <v>4</v>
@@ -2976,13 +3183,21 @@
       <c r="F12" s="5">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C13" s="2">
         <v>3</v>
@@ -2996,13 +3211,21 @@
       <c r="F13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C14" s="6">
         <v>208</v>
@@ -3015,12 +3238,34 @@
       </c>
       <c r="F14" s="7">
         <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>33.39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16">
+        <f>SUM(H2:H15)</f>
+        <v>82.51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <conditionalFormatting sqref="A2:H14">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$G2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>